<commit_message>
added melckenburg vorpommern staedte
</commit_message>
<xml_diff>
--- a/data/municipal_elections/archive/final_output/Sources_overview.xlsx
+++ b/data/municipal_elections/archive/final_output/Sources_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Library/CloudStorage/Dropbox/RA_work/Data collection/Germany_Kommunalwahlen/final_output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/archive/final_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE98511-B35B-3C47-977E-42973F8970AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E8E18A-FA99-6849-B820-B5852E0FD39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4380" yWindow="-21100" windowWidth="38400" windowHeight="20200" xr2:uid="{226FADFE-BBFE-E444-B07F-A513505EA323}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +605,7 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
@@ -676,6 +676,7 @@
     <hyperlink ref="B8" r:id="rId1" tooltip="https://statistik.hessen.de/zahlen-fakten/kommunalwahlen" xr:uid="{1D9A2FC2-8512-9942-8F8F-397AE5277A7F}"/>
     <hyperlink ref="B16" r:id="rId2" xr:uid="{4A0ED774-FE99-8D40-B9A8-0DBDBA3E8538}"/>
     <hyperlink ref="B17" r:id="rId3" xr:uid="{8DFB7A3C-FD70-EC48-AB8E-6D29204472F8}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{E52DB018-FC44-4D4E-8A00-082386D2CF51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>